<commit_message>
Add Helm chart templates and configuration files
</commit_message>
<xml_diff>
--- a/bench/bench.xlsx
+++ b/bench/bench.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>unsecure local</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>insecure CXL</t>
-  </si>
-  <si>
-    <t>xts local</t>
   </si>
   <si>
     <t>xts ide</t>
@@ -84,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,12 +88,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -138,27 +126,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -469,19 +454,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -495,359 +478,263 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1.092130329</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1.028489199</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.161274809</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.104731474</v>
       </c>
       <c r="E2" s="4">
-        <v>1.26826344</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1.206510749</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1.105458599</v>
+        <v>1.012203919</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1.333568505</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1.13767486</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.308986074</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.494567785</v>
       </c>
       <c r="E3" s="4">
-        <v>1.745622601</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1.993108526</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1.453904964</v>
+        <v>1.090236429</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1.088160127</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.03551061</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.099614326</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.072693569</v>
       </c>
       <c r="E4" s="4">
-        <v>1.196556465</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.16726237</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1.124948148</v>
+        <v>1.033807544</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1.130401526</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1.043732136</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.14153328</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.207673945</v>
       </c>
       <c r="E5" s="4">
-        <v>1.290390962</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.365156471</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1.192757356</v>
+        <v>1.055162549</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1.09108663</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1.041428053</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.091700095</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.142609235</v>
       </c>
       <c r="E6" s="4">
-        <v>1.191139377</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1.24668566</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1.138915041</v>
+        <v>1.043835576</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1.34762654</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1.133774339</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.31013832</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.466768421</v>
       </c>
       <c r="E7" s="4">
-        <v>1.765577172</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1.976656053</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1.384128258</v>
+        <v>1.02708593</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.315076905</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.437949679</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.041254523</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.329159101</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.514382146</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.098631253</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1.345788055</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.142010465</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.769814791</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1.935175502</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.4013079</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="6" t="s">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.294815677</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.283692392</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.099535309</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1.371738932</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.152388511</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.823259286</v>
-      </c>
-      <c r="F9" s="4">
-        <v>2.077336948</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1.507035262</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="6" t="s">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.315653217</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.509595651</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.045333561</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1.306774944</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1.124949033</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1.692032684</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1.677497054</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1.436845192</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="6" t="s">
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.185717845</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.230712826</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.008141428</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1.355009321</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1.152369746</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1.782722372</v>
-      </c>
-      <c r="F11" s="4">
-        <v>2.045516178</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1.416436718</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="7" t="s">
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.00668373</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.009831201</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.003453528</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1.168893763</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.062294492</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1.385978194</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1.438572547</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1.178410228</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="7" t="s">
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.250929555</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.20201772</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.056774722</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1.005298063</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.002408025</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1.012571855</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1.013707792</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1.009263867</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1.235979767</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1.097996277</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1.54612362</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1.485669581</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1.306152175</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1.097840269</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1.040300414</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1.217850187</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1.255645937</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1.156801441</v>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.099915486</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.081892471</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.045862188</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1.212164055</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1.08538044</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.207942744</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.268508465</v>
       </c>
       <c r="E16" s="4">
-        <v>1.477707358</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1.563178669</v>
-      </c>
-      <c r="G16" s="5">
-        <v>1.272311796</v>
+        <v>1.047237033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new benchmark files for multicore testing
</commit_message>
<xml_diff>
--- a/bench/bench.xlsx
+++ b/bench/bench.xlsx
@@ -14,18 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>insecure CXL</t>
-  </si>
-  <si>
-    <t>xts ide</t>
-  </si>
-  <si>
-    <t>ctr ide (new)</t>
-  </si>
-  <si>
-    <t>adpative(updated)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Adaptive</t>
+  </si>
+  <si>
+    <t>CTR +GCM -SC</t>
+  </si>
+  <si>
+    <t>CTR +GCM +SC</t>
+  </si>
+  <si>
+    <t>CL +GCM -ECC</t>
+  </si>
+  <si>
+    <t>CL +GCM +ECC</t>
+  </si>
+  <si>
+    <t>XTS +GCM</t>
+  </si>
+  <si>
+    <t>Insecure CXL</t>
   </si>
   <si>
     <t>605.mcf_s</t>
@@ -78,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +104,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -126,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -137,7 +152,13 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -454,20 +475,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -478,263 +502,407 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>1.161274809</v>
+        <v>1.016543126</v>
       </c>
       <c r="D2" s="3">
-        <v>1.104731474</v>
+        <v>1.162441731</v>
       </c>
       <c r="E2" s="4">
-        <v>1.012203919</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+        <v>1.16180676</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1.348877576</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1.163015946</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>1.308986074</v>
+        <v>1.094763133</v>
       </c>
       <c r="D3" s="3">
-        <v>1.494567785</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.090236429</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+        <v>1.393109534</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.31064719</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1.561669751</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1.337460075</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4" s="3">
-        <v>1.099614326</v>
+        <v>1.033040115</v>
       </c>
       <c r="D4" s="3">
-        <v>1.072693569</v>
+        <v>1.086300821</v>
       </c>
       <c r="E4" s="4">
-        <v>1.033807544</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+        <v>1.103262491</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1.185900793</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1.102452675</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5" s="3">
-        <v>1.14153328</v>
+        <v>1.060243844</v>
       </c>
       <c r="D5" s="3">
-        <v>1.207673945</v>
+        <v>1.188495713</v>
       </c>
       <c r="E5" s="4">
-        <v>1.055162549</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+        <v>1.147426489</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.265392448</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1.153604421</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
         <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>1.091700095</v>
+        <v>1.034139717</v>
       </c>
       <c r="D6" s="3">
-        <v>1.142609235</v>
+        <v>1.150128062</v>
       </c>
       <c r="E6" s="4">
-        <v>1.043835576</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+        <v>1.090589884</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.168811422</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1.094118577</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
         <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>1.31013832</v>
+        <v>1.023732013</v>
       </c>
       <c r="D7" s="3">
-        <v>1.466768421</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.02708593</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+        <v>1.324602655</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.314294718</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1.534565251</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1.334723117</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>1.315076905</v>
+        <v>1.043533493</v>
       </c>
       <c r="D8" s="3">
-        <v>1.437949679</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.041254523</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>1.349823588</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1.318906015</v>
+      </c>
+      <c r="F8" s="6">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.559879302</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1.323249897</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="3">
-        <v>1.329159101</v>
+        <v>1.095298366</v>
       </c>
       <c r="D9" s="3">
-        <v>1.514382146</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.098631253</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="5" t="s">
-        <v>12</v>
+        <v>1.423268963</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.340147538</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1.619578166</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1.34660601</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>1.294815677</v>
+        <v>1.096680844</v>
       </c>
       <c r="D10" s="3">
-        <v>1.283692392</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.099535309</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>1.40161791</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1.298694438</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.599545546</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.309857163</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>1.315653217</v>
+        <v>1.041297922</v>
       </c>
       <c r="D11" s="3">
-        <v>1.509595651</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1.045333561</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>1.359189507</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.319252448</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.547682589</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1.335875084</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>1.185717845</v>
+        <v>1.000782359</v>
       </c>
       <c r="D12" s="3">
-        <v>1.230712826</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1.008141428</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
+        <v>1.14026877</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.183029518</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1.306266715</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.191421874</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="3">
-        <v>1.00668373</v>
+        <v>1.003428081</v>
       </c>
       <c r="D13" s="3">
-        <v>1.009831201</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1.003453528</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="6" t="s">
-        <v>16</v>
+        <v>1.008921324</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.006758867</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1.015262571</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1.007713799</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
       <c r="C14" s="3">
-        <v>1.250929555</v>
+        <v>1.062439549</v>
       </c>
       <c r="D14" s="3">
-        <v>1.20201772</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1.056774722</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="6" t="s">
-        <v>17</v>
+        <v>1.342720808</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.24644814</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1.589612765</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.280191379</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>1.099915486</v>
+        <v>1.04465276</v>
       </c>
       <c r="D15" s="3">
-        <v>1.081892471</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1.045862188</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+        <v>1.150955945</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.100528976</v>
+      </c>
+      <c r="F15" s="6">
+        <v>2</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1.203983006</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1.115413319</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="4">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5">
         <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>1.207942744</v>
+        <v>1.046469666</v>
       </c>
       <c r="D16" s="3">
-        <v>1.268508465</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1.047237033</v>
+        <v>1.248703238</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.210128105</v>
+      </c>
+      <c r="F16" s="6">
+        <v>2</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1.393359136</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1.221121667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>